<commit_message>
Am terminat Obiective + Structura Lucrarii
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4515E567-5B26-478B-8E34-90163CDEF229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFFE7EB-EDD7-4FBA-9F81-8F76B8C7B445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Day</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Introducere (Context + Problema + Obiective aproape</t>
+  </si>
+  <si>
+    <t>Am terminat Obiective + Structura Lucrarii</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -438,14 +441,26 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45449</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45479</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
@@ -511,7 +526,7 @@
       </c>
       <c r="D16" s="4">
         <f>SUM(C3:C13)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4">

</xml_diff>

<commit_message>
1/2 of section 6
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C379F575-5253-4490-9D90-CB127EFDABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB601BD0-4FF2-4951-A67C-61FE13A0032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Terminare concluzie</t>
+  </si>
+  <si>
+    <t>Terminare jumatate din capitolul 6</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -507,9 +510,15 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="2">
+        <v>45541</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1"/>
@@ -555,7 +564,7 @@
       </c>
       <c r="D16" s="4">
         <f>SUM(C3:C13)</f>
-        <v>16.850000000000001</v>
+        <v>20.85</v>
       </c>
     </row>
     <row r="17" spans="1:4">

</xml_diff>

<commit_message>
finished refactor for section 6, 7, 8
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7AF05-EA2E-4A8B-8F0C-BD0288518E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7DCC90-E0AA-49A6-BC67-EF78CED2B150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Day</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Refactorizare capitolul 1</t>
+  </si>
+  <si>
+    <t>15/6/2024</t>
+  </si>
+  <si>
+    <t>Refactorizare capitolul 6, 7, 8</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -558,9 +564,15 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
@@ -588,7 +600,7 @@
       </c>
       <c r="D16" s="4">
         <f>SUM(C3:C13)</f>
-        <v>27.51</v>
+        <v>30.51</v>
       </c>
     </row>
     <row r="17" spans="1:4">

</xml_diff>

<commit_message>
finished refactor for section 2, 3
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7DCC90-E0AA-49A6-BC67-EF78CED2B150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED410103-556C-4395-A9B1-AD5B9D9BACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Day</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Refactorizare capitolul 6, 7, 8</t>
+  </si>
+  <si>
+    <t>Refactorizare capitolul 2, 3</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -577,8 +580,12 @@
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1"/>
@@ -600,7 +607,7 @@
       </c>
       <c r="D16" s="4">
         <f>SUM(C3:C13)</f>
-        <v>30.51</v>
+        <v>32.010000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:4">

</xml_diff>

<commit_message>
made bookmark for 4 and 5 + finished 4.1
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED410103-556C-4395-A9B1-AD5B9D9BACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8BB90C-5A1D-4AB8-9C5E-F4484AE99C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Day</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Refactorizare capitolul 2, 3</t>
+  </si>
+  <si>
+    <t>16/6/2024</t>
+  </si>
+  <si>
+    <t>Creare curpins pentru capitolele 4 si 5 + Finalizare 4.1</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -588,10 +594,18 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
@@ -600,32 +614,50 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="4">
-        <f>SUM(C3:C13)</f>
-        <v>32.010000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
+      <c r="D19" s="4">
+        <f>SUM(C3:C18)</f>
+        <v>35.340000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finsihed 4.2 with all the diagrams, etc
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8BB90C-5A1D-4AB8-9C5E-F4484AE99C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD382840-774C-42DD-9A6E-C3944F3DAA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Day</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Creare curpins pentru capitolele 4 si 5 + Finalizare 4.1</t>
+  </si>
+  <si>
+    <t>Finalizare 4.2 cu diagrame si nebunii</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,12 @@
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
@@ -639,7 +646,7 @@
       </c>
       <c r="D19" s="4">
         <f>SUM(C3:C18)</f>
-        <v>35.340000000000003</v>
+        <v>41.84</v>
       </c>
     </row>
     <row r="20" spans="1:4">

</xml_diff>

<commit_message>
finished section 5.1, 5.2
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B87668-DB87-4CD0-B149-0A050E0EEFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9647B-5961-45F6-885F-4CB993BBC309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Day</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Finalizare intreg capitolul 4</t>
+  </si>
+  <si>
+    <t>Finalizare 5.1 si 5.2</t>
+  </si>
+  <si>
+    <t>18/6/2024</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -641,10 +647,18 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="1">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
@@ -653,32 +667,56 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="4">
-        <f>SUM(C3:C18)</f>
-        <v>46.84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
+      <c r="D23" s="4">
+        <f>SUM(C3:C22)</f>
+        <v>50.14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished everything, no refactoring yet
</commit_message>
<xml_diff>
--- a/files/documentation/Documentatie - Timeline.xlsx
+++ b/files/documentation/Documentatie - Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5D1A0-9FD3-4E27-8E41-FA1B0C359E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F690D05-9ECA-4E41-9051-B845CAB472E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Day</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Finalizat aproape tot</t>
+  </si>
+  <si>
+    <t>Finalizat tot, mai ramane doar o ultima refactorizare</t>
+  </si>
+  <si>
+    <t>19/6/2024</t>
   </si>
 </sst>
 </file>
@@ -445,7 +451,7 @@
   <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -674,10 +680,18 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1"/>
@@ -705,7 +719,7 @@
       </c>
       <c r="D23" s="4">
         <f>SUM(C3:C22)</f>
-        <v>52.94</v>
+        <v>54.19</v>
       </c>
     </row>
     <row r="24" spans="1:4">

</xml_diff>